<commit_message>
xlsx fixed and tweet style added
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickschmeiter/Downloads/Bachelorthesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4132C8-7C22-AD4C-A05D-88CC92CF9527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744F1FB6-6FC7-C142-8F4F-81321B11A84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31600" yWindow="8140" windowWidth="28040" windowHeight="17440" xr2:uid="{03E4B43B-A708-C046-B26F-2C195EF0064C}"/>
+    <workbookView xWindow="-34560" yWindow="5060" windowWidth="34560" windowHeight="21600" xr2:uid="{03E4B43B-A708-C046-B26F-2C195EF0064C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="198">
   <si>
     <t>username</t>
   </si>
@@ -207,6 +207,429 @@
   </si>
   <si>
     <t>cars, planes, trains, HSV</t>
+  </si>
+  <si>
+    <t>diddykong</t>
+  </si>
+  <si>
+    <t>half brazilien half german</t>
+  </si>
+  <si>
+    <t>translator</t>
+  </si>
+  <si>
+    <t>anime, hiking</t>
+  </si>
+  <si>
+    <t>Munich</t>
+  </si>
+  <si>
+    <t>djpete</t>
+  </si>
+  <si>
+    <t>dj</t>
+  </si>
+  <si>
+    <t>techno, cooking, meditation</t>
+  </si>
+  <si>
+    <t>democratic</t>
+  </si>
+  <si>
+    <t>lisalieb</t>
+  </si>
+  <si>
+    <t>Stuttgart</t>
+  </si>
+  <si>
+    <t>political sciences student</t>
+  </si>
+  <si>
+    <t>politics</t>
+  </si>
+  <si>
+    <t>Cologne</t>
+  </si>
+  <si>
+    <t>coldwarmmirror</t>
+  </si>
+  <si>
+    <t>half polish half german</t>
+  </si>
+  <si>
+    <t>content creator on youtube</t>
+  </si>
+  <si>
+    <t>movies, books</t>
+  </si>
+  <si>
+    <t>center</t>
+  </si>
+  <si>
+    <t>shanghaistinker</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>skateboarding, modelling, playing bass</t>
+  </si>
+  <si>
+    <t>berlin</t>
+  </si>
+  <si>
+    <t>KIZMico</t>
+  </si>
+  <si>
+    <t>rapper</t>
+  </si>
+  <si>
+    <t>climate, rap, graffiti</t>
+  </si>
+  <si>
+    <t>left extreme</t>
+  </si>
+  <si>
+    <t>Blaubärin</t>
+  </si>
+  <si>
+    <t>Social Media Marketing</t>
+  </si>
+  <si>
+    <t>books, kid tv shows, tv shows</t>
+  </si>
+  <si>
+    <t>liberal</t>
+  </si>
+  <si>
+    <t>Montelover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">half german half russian </t>
+  </si>
+  <si>
+    <t>high school student</t>
+  </si>
+  <si>
+    <t>youtube, soccer</t>
+  </si>
+  <si>
+    <t>Village in bavaria</t>
+  </si>
+  <si>
+    <t>Village in North rine westphalia</t>
+  </si>
+  <si>
+    <t>CrazyCatWoman</t>
+  </si>
+  <si>
+    <t>jobless</t>
+  </si>
+  <si>
+    <t>cats, the simpsons</t>
+  </si>
+  <si>
+    <t>village in Saxony</t>
+  </si>
+  <si>
+    <t>ichesselicht</t>
+  </si>
+  <si>
+    <t>non binary</t>
+  </si>
+  <si>
+    <t>works in school for disabled people</t>
+  </si>
+  <si>
+    <t>south park, books, mental diseases</t>
+  </si>
+  <si>
+    <t>Sophiesm</t>
+  </si>
+  <si>
+    <t>dutch</t>
+  </si>
+  <si>
+    <t>feminism, computer science</t>
+  </si>
+  <si>
+    <t>ebossa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">half norwegien half german </t>
+  </si>
+  <si>
+    <t>painter</t>
+  </si>
+  <si>
+    <t>art, travelling</t>
+  </si>
+  <si>
+    <t>vivlvivi</t>
+  </si>
+  <si>
+    <t>software developer</t>
+  </si>
+  <si>
+    <t>trash tv, pottery, rap</t>
+  </si>
+  <si>
+    <t>sigsig</t>
+  </si>
+  <si>
+    <t>data scientist</t>
+  </si>
+  <si>
+    <t>indie rock, billiard, skateboarding</t>
+  </si>
+  <si>
+    <t>Molona</t>
+  </si>
+  <si>
+    <t>techno, literature</t>
+  </si>
+  <si>
+    <t>german teacher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Berlin </t>
+  </si>
+  <si>
+    <t>relerelu</t>
+  </si>
+  <si>
+    <t>finance, shares</t>
+  </si>
+  <si>
+    <t>godonskis</t>
+  </si>
+  <si>
+    <t>half austrian half german</t>
+  </si>
+  <si>
+    <t>ski teacher</t>
+  </si>
+  <si>
+    <t>skiing, snowboarding</t>
+  </si>
+  <si>
+    <t>tonysoprano</t>
+  </si>
+  <si>
+    <t>drug dealer</t>
+  </si>
+  <si>
+    <t>tv shows, books, criminal stuff</t>
+  </si>
+  <si>
+    <t>racingluke</t>
+  </si>
+  <si>
+    <t>100m runner</t>
+  </si>
+  <si>
+    <t>sports, running, astrology</t>
+  </si>
+  <si>
+    <t>steffsteff</t>
+  </si>
+  <si>
+    <t>architect</t>
+  </si>
+  <si>
+    <t>art, architecture, languages</t>
+  </si>
+  <si>
+    <t>marlonma</t>
+  </si>
+  <si>
+    <t>consultant</t>
+  </si>
+  <si>
+    <t>watches, cars, finance</t>
+  </si>
+  <si>
+    <t>realtim</t>
+  </si>
+  <si>
+    <t>half british half italian</t>
+  </si>
+  <si>
+    <t>employee of german tax government</t>
+  </si>
+  <si>
+    <t>beer, soccer, finances</t>
+  </si>
+  <si>
+    <t>rrrrrhos</t>
+  </si>
+  <si>
+    <t>manager in Tech</t>
+  </si>
+  <si>
+    <t>politics, cars</t>
+  </si>
+  <si>
+    <t>very conservative</t>
+  </si>
+  <si>
+    <t>junkyjunk</t>
+  </si>
+  <si>
+    <t>junkyard worker</t>
+  </si>
+  <si>
+    <t>cars, mechanical engineering</t>
+  </si>
+  <si>
+    <t>village close to Hamburg</t>
+  </si>
+  <si>
+    <t>florobo</t>
+  </si>
+  <si>
+    <t>horses</t>
+  </si>
+  <si>
+    <t>taralala</t>
+  </si>
+  <si>
+    <t>teergießer</t>
+  </si>
+  <si>
+    <t>half japanese half german</t>
+  </si>
+  <si>
+    <t>construction worker</t>
+  </si>
+  <si>
+    <t>cooking, anime, Ballet</t>
+  </si>
+  <si>
+    <t>nevernude</t>
+  </si>
+  <si>
+    <t>half german half swedish</t>
+  </si>
+  <si>
+    <t>stripper</t>
+  </si>
+  <si>
+    <t>woman rights, tv shows, weed</t>
+  </si>
+  <si>
+    <t>brokenhearts</t>
+  </si>
+  <si>
+    <t>half german half taiwanese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prostitute </t>
+  </si>
+  <si>
+    <t>techno, dogs, travelling</t>
+  </si>
+  <si>
+    <t>julujonas</t>
+  </si>
+  <si>
+    <t>Asian studies student</t>
+  </si>
+  <si>
+    <t>anime, languages</t>
+  </si>
+  <si>
+    <t>Duisburg</t>
+  </si>
+  <si>
+    <t>rap, anime</t>
+  </si>
+  <si>
+    <t>left liberal</t>
+  </si>
+  <si>
+    <t>mariemara</t>
+  </si>
+  <si>
+    <t>newerakid</t>
+  </si>
+  <si>
+    <t>product marketing student</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fashion, hip hop </t>
+  </si>
+  <si>
+    <t xml:space="preserve">berlin </t>
+  </si>
+  <si>
+    <t>rraluca19</t>
+  </si>
+  <si>
+    <t>polish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">economics student </t>
+  </si>
+  <si>
+    <t>formula 1, soccer</t>
+  </si>
+  <si>
+    <t>maximmongus</t>
+  </si>
+  <si>
+    <t>supermarket employee</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cinema, photography</t>
+  </si>
+  <si>
+    <t>aarolono</t>
+  </si>
+  <si>
+    <t>history teacher student</t>
+  </si>
+  <si>
+    <t>video games, history</t>
+  </si>
+  <si>
+    <t>Münster</t>
+  </si>
+  <si>
+    <t>barapara</t>
+  </si>
+  <si>
+    <t>philosophy and art student</t>
+  </si>
+  <si>
+    <t>trading card games, video games</t>
+  </si>
+  <si>
+    <t>ThisisKIKI</t>
+  </si>
+  <si>
+    <t>DJ</t>
+  </si>
+  <si>
+    <t>Techno, Yoga</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>jensbenz</t>
+  </si>
+  <si>
+    <t>mercedes benz, hip hop</t>
+  </si>
+  <si>
+    <t>belugazucker</t>
+  </si>
+  <si>
+    <t>biologist</t>
+  </si>
+  <si>
+    <t>whaley, sea, climate change</t>
   </si>
 </sst>
 </file>
@@ -578,14 +1001,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A37ED32-125B-4D4D-9C83-0685CA6F2F16}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="4" max="4" width="27.5" customWidth="1"/>
     <col min="5" max="5" width="30.6640625" customWidth="1"/>
     <col min="6" max="6" width="25.83203125" customWidth="1"/>
     <col min="8" max="8" width="20.6640625" customWidth="1"/>
@@ -903,6 +1327,1020 @@
         <v>51</v>
       </c>
     </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" t="s">
+        <v>97</v>
+      </c>
+      <c r="H21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" t="s">
+        <v>93</v>
+      </c>
+      <c r="H23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" t="s">
+        <v>108</v>
+      </c>
+      <c r="G24" t="s">
+        <v>79</v>
+      </c>
+      <c r="H24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>110</v>
+      </c>
+      <c r="F25" t="s">
+        <v>111</v>
+      </c>
+      <c r="G25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" t="s">
+        <v>114</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>117</v>
+      </c>
+      <c r="F27" t="s">
+        <v>116</v>
+      </c>
+      <c r="G27" t="s">
+        <v>118</v>
+      </c>
+      <c r="H27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" t="s">
+        <v>120</v>
+      </c>
+      <c r="G28" t="s">
+        <v>61</v>
+      </c>
+      <c r="H28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>121</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>122</v>
+      </c>
+      <c r="E29" t="s">
+        <v>123</v>
+      </c>
+      <c r="F29" t="s">
+        <v>124</v>
+      </c>
+      <c r="G29" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30">
+        <v>22</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>126</v>
+      </c>
+      <c r="F30" t="s">
+        <v>127</v>
+      </c>
+      <c r="G30" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>128</v>
+      </c>
+      <c r="B31">
+        <v>24</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>129</v>
+      </c>
+      <c r="F31" t="s">
+        <v>130</v>
+      </c>
+      <c r="G31" t="s">
+        <v>61</v>
+      </c>
+      <c r="H31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32">
+        <v>26</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>132</v>
+      </c>
+      <c r="F32" t="s">
+        <v>133</v>
+      </c>
+      <c r="G32" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33">
+        <v>29</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>135</v>
+      </c>
+      <c r="F33" t="s">
+        <v>136</v>
+      </c>
+      <c r="G33" t="s">
+        <v>50</v>
+      </c>
+      <c r="H33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>137</v>
+      </c>
+      <c r="B34">
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>138</v>
+      </c>
+      <c r="E34" t="s">
+        <v>139</v>
+      </c>
+      <c r="F34" t="s">
+        <v>140</v>
+      </c>
+      <c r="G34" t="s">
+        <v>67</v>
+      </c>
+      <c r="H34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>141</v>
+      </c>
+      <c r="B35">
+        <v>53</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>142</v>
+      </c>
+      <c r="F35" t="s">
+        <v>143</v>
+      </c>
+      <c r="G35" t="s">
+        <v>61</v>
+      </c>
+      <c r="H35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>145</v>
+      </c>
+      <c r="B36">
+        <v>21</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" t="s">
+        <v>146</v>
+      </c>
+      <c r="F36" t="s">
+        <v>147</v>
+      </c>
+      <c r="G36" t="s">
+        <v>148</v>
+      </c>
+      <c r="H36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>149</v>
+      </c>
+      <c r="B37">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F37" t="s">
+        <v>150</v>
+      </c>
+      <c r="G37" t="s">
+        <v>50</v>
+      </c>
+      <c r="H37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>151</v>
+      </c>
+      <c r="B38">
+        <v>16</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" t="s">
+        <v>90</v>
+      </c>
+      <c r="F38" t="s">
+        <v>150</v>
+      </c>
+      <c r="G38" t="s">
+        <v>61</v>
+      </c>
+      <c r="H38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>152</v>
+      </c>
+      <c r="B39">
+        <v>19</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" t="s">
+        <v>153</v>
+      </c>
+      <c r="E39" t="s">
+        <v>154</v>
+      </c>
+      <c r="F39" t="s">
+        <v>155</v>
+      </c>
+      <c r="G39" t="s">
+        <v>93</v>
+      </c>
+      <c r="H39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>156</v>
+      </c>
+      <c r="B40">
+        <v>22</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" t="s">
+        <v>157</v>
+      </c>
+      <c r="E40" t="s">
+        <v>158</v>
+      </c>
+      <c r="F40" t="s">
+        <v>159</v>
+      </c>
+      <c r="G40" t="s">
+        <v>79</v>
+      </c>
+      <c r="H40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>160</v>
+      </c>
+      <c r="B41">
+        <v>23</v>
+      </c>
+      <c r="C41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" t="s">
+        <v>161</v>
+      </c>
+      <c r="E41" t="s">
+        <v>162</v>
+      </c>
+      <c r="F41" t="s">
+        <v>163</v>
+      </c>
+      <c r="G41" t="s">
+        <v>50</v>
+      </c>
+      <c r="H41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>164</v>
+      </c>
+      <c r="B42">
+        <v>26</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" t="s">
+        <v>165</v>
+      </c>
+      <c r="F42" t="s">
+        <v>166</v>
+      </c>
+      <c r="G42" t="s">
+        <v>167</v>
+      </c>
+      <c r="H42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>170</v>
+      </c>
+      <c r="B43">
+        <v>17</v>
+      </c>
+      <c r="C43" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" t="s">
+        <v>90</v>
+      </c>
+      <c r="F43" t="s">
+        <v>168</v>
+      </c>
+      <c r="G43" t="s">
+        <v>148</v>
+      </c>
+      <c r="H43" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>171</v>
+      </c>
+      <c r="B44">
+        <v>22</v>
+      </c>
+      <c r="C44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" t="s">
+        <v>172</v>
+      </c>
+      <c r="F44" t="s">
+        <v>173</v>
+      </c>
+      <c r="G44" t="s">
+        <v>174</v>
+      </c>
+      <c r="H44" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>175</v>
+      </c>
+      <c r="B45">
+        <v>21</v>
+      </c>
+      <c r="C45" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" t="s">
+        <v>176</v>
+      </c>
+      <c r="E45" t="s">
+        <v>177</v>
+      </c>
+      <c r="F45" t="s">
+        <v>178</v>
+      </c>
+      <c r="G45" t="s">
+        <v>79</v>
+      </c>
+      <c r="H45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>179</v>
+      </c>
+      <c r="B46">
+        <v>20</v>
+      </c>
+      <c r="C46" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" t="s">
+        <v>180</v>
+      </c>
+      <c r="F46" t="s">
+        <v>181</v>
+      </c>
+      <c r="G46" t="s">
+        <v>79</v>
+      </c>
+      <c r="H46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>182</v>
+      </c>
+      <c r="B47">
+        <v>23</v>
+      </c>
+      <c r="C47" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" t="s">
+        <v>183</v>
+      </c>
+      <c r="F47" t="s">
+        <v>184</v>
+      </c>
+      <c r="G47" t="s">
+        <v>185</v>
+      </c>
+      <c r="H47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>186</v>
+      </c>
+      <c r="B48">
+        <v>25</v>
+      </c>
+      <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" t="s">
+        <v>187</v>
+      </c>
+      <c r="F48" t="s">
+        <v>188</v>
+      </c>
+      <c r="G48" t="s">
+        <v>185</v>
+      </c>
+      <c r="H48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>189</v>
+      </c>
+      <c r="B49">
+        <v>28</v>
+      </c>
+      <c r="C49" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>190</v>
+      </c>
+      <c r="F49" t="s">
+        <v>191</v>
+      </c>
+      <c r="G49" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>193</v>
+      </c>
+      <c r="B50">
+        <v>25</v>
+      </c>
+      <c r="C50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" t="s">
+        <v>55</v>
+      </c>
+      <c r="F50" t="s">
+        <v>194</v>
+      </c>
+      <c r="G50" t="s">
+        <v>67</v>
+      </c>
+      <c r="H50" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>195</v>
+      </c>
+      <c r="B51">
+        <v>28</v>
+      </c>
+      <c r="C51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" t="s">
+        <v>196</v>
+      </c>
+      <c r="F51" t="s">
+        <v>197</v>
+      </c>
+      <c r="G51" t="s">
+        <v>61</v>
+      </c>
+      <c r="H51" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>